<commit_message>
update assign student course
</commit_message>
<xml_diff>
--- a/Documents/COMP1640 Group04 CMS Sprint03.xlsx
+++ b/Documents/COMP1640 Group04 CMS Sprint03.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Task</t>
   </si>
@@ -67,19 +67,16 @@
     <t>Manage StudentCourses</t>
   </si>
   <si>
-    <t>Students Testing</t>
-  </si>
-  <si>
     <t>Faculties Test</t>
   </si>
   <si>
     <t>Manage Faculties</t>
   </si>
   <si>
-    <t>FacultyCourses Testing</t>
+    <t>Students Test</t>
   </si>
   <si>
-    <t>StudentCourses Test</t>
+    <t>FucultyCourses Test</t>
   </si>
 </sst>
 </file>
@@ -290,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -400,25 +397,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="53">
     <dxf>
       <font>
         <color rgb="FF003366"/>
@@ -595,6 +580,282 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFFF6600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFADCB3"/>
+          <bgColor rgb="FFFADCB3"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCC00"/>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF003366"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFCC"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF6600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFADCB3"/>
+          <bgColor rgb="FFFADCB3"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCC00"/>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF003366"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFCC"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF6600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFADCB3"/>
+          <bgColor rgb="FFFADCB3"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCC00"/>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF003366"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFCC"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF6600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFADCB3"/>
+          <bgColor rgb="FFFADCB3"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCC00"/>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF003366"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFCC"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF800000"/>
       </font>
       <fill>
@@ -742,6 +1003,297 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFCCFFCC"/>
           <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF003366"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFCC"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF6600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFADCB3"/>
+          <bgColor rgb="FFFADCB3"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCC00"/>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF003366"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFCC"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF6600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFADCB3"/>
+          <bgColor rgb="FFFADCB3"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCC00"/>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF003366"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFCC"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF6600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFADCB3"/>
+          <bgColor rgb="FFFADCB3"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCC00"/>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF003366"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFFF"/>
+          <bgColor rgb="FFCCFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF008000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFCC"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF6600"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFADCB3"/>
+          <bgColor rgb="FFFADCB3"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCC00"/>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="1"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCC00"/>
+          <bgColor rgb="FFFFCC00"/>
         </patternFill>
       </fill>
       <alignment wrapText="1"/>
@@ -774,7 +1326,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.4012928136049117E-2"/>
+          <c:y val="0.13722962847465847"/>
+          <c:w val="0.871909936877725"/>
+          <c:h val="0.6416188075500463"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="1"/>
@@ -783,7 +1345,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$16</c:f>
+              <c:f>Sheet1!$C$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -804,45 +1366,102 @@
           </c:marker>
           <c:cat>
             <c:numRef>
+              <c:f>Sheet1!$D$14:$S$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
               <c:f>Sheet1!$D$15:$S$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>34</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>6</c:v>
@@ -855,63 +1474,6 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$16:$S$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -929,45 +1491,45 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$15:$S$15</c:f>
+              <c:f>Sheet1!$D$14:$S$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>6</c:v>
@@ -1119,13 +1681,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1411,13 +1973,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S79"/>
+  <dimension ref="A1:S78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1524,11 +2086,11 @@
         <v>6</v>
       </c>
       <c r="C3" s="7">
-        <f t="shared" ref="C3:C11" si="0">IF(B3&lt;SUM(E3:S3),SUM(E3:S3),B3)</f>
+        <f>IF(B3&lt;SUM(E3:S3),SUM(E3:S3),B3)</f>
         <v>6</v>
       </c>
       <c r="D3" s="8">
-        <f t="shared" ref="D3:D11" si="1">IF(C3&gt;B3,$C3-(SUM($E3:$S3)),$B3-(SUM($E3:$S3)))</f>
+        <f>IF(C3&gt;B3,$C3-(SUM($E3:$S3)),$B3-(SUM($E3:$S3)))</f>
         <v>0</v>
       </c>
       <c r="E3" s="9">
@@ -1559,11 +2121,11 @@
         <v>4</v>
       </c>
       <c r="C4" s="7">
-        <f t="shared" si="0"/>
+        <f>IF(B4&lt;SUM(E4:S4),SUM(E4:S4),B4)</f>
         <v>4</v>
       </c>
       <c r="D4" s="8">
-        <f t="shared" si="1"/>
+        <f>IF(C4&gt;B4,$C4-(SUM($E4:$S4)),$B4-(SUM($E4:$S4)))</f>
         <v>0</v>
       </c>
       <c r="E4" s="12"/>
@@ -1580,65 +2142,91 @@
         <v>10</v>
       </c>
       <c r="C5" s="7">
-        <f t="shared" si="0"/>
+        <f>IF(B5&lt;SUM(E5:S5),SUM(E5:S5),B5)</f>
         <v>10</v>
       </c>
       <c r="D5" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f>IF(C5&gt;B5,$C5-(SUM($E5:$S5)),$B5-(SUM($E5:$S5)))</f>
+        <v>0</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I5">
         <v>2</v>
       </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
     </row>
     <row r="6" spans="1:19" s="33" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
+        <v>19</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7">
+        <f>IF(B6&lt;SUM(E6:S6),SUM(E6:S6),B6)</f>
+        <v>2</v>
+      </c>
+      <c r="D6" s="8">
+        <f>IF(C6&gt;B6,$C6-(SUM($E6:$S6)),$B6-(SUM($E6:$S6)))</f>
+        <v>0</v>
+      </c>
       <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
       <c r="H6" s="13"/>
+      <c r="J6" s="33">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="6">
         <v>10</v>
       </c>
       <c r="C7" s="7">
-        <f t="shared" si="0"/>
+        <f>IF(B7&lt;SUM(E7:S7),SUM(E7:S7),B7)</f>
         <v>10</v>
       </c>
       <c r="D7" s="8">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f>IF(C7&gt;B7,$C7-(SUM($E7:$S7)),$B7-(SUM($E7:$S7)))</f>
+        <v>0</v>
       </c>
       <c r="E7" s="12"/>
       <c r="H7" s="13"/>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:19" s="33" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
+        <v>17</v>
+      </c>
+      <c r="B8" s="6">
+        <v>2</v>
+      </c>
+      <c r="C8" s="7">
+        <f>IF(B8&lt;SUM(E8:S8),SUM(E8:S8),B8)</f>
+        <v>2</v>
+      </c>
+      <c r="D8" s="8">
+        <f>IF(C8&gt;B8,$C8-(SUM($E8:$S8)),$B8-(SUM($E8:$S8)))</f>
+        <v>0</v>
+      </c>
       <c r="E8" s="12"/>
       <c r="H8" s="13"/>
+      <c r="L8" s="33">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:19" s="32" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -1648,25 +2236,45 @@
         <v>10</v>
       </c>
       <c r="C9" s="7">
-        <f t="shared" si="0"/>
+        <f>IF(B9&lt;SUM(E9:S9),SUM(E9:S9),B9)</f>
         <v>10</v>
       </c>
       <c r="D9" s="8">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f>IF(C9&gt;B9,$C9-(SUM($E9:$S9)),$B9-(SUM($E9:$S9)))</f>
+        <v>0</v>
       </c>
       <c r="E9" s="12"/>
       <c r="H9" s="13"/>
+      <c r="M9" s="32">
+        <v>4</v>
+      </c>
+      <c r="N9" s="32">
+        <v>4</v>
+      </c>
+      <c r="O9" s="32">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:19" s="33" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
+      <c r="B10" s="6">
+        <v>2</v>
+      </c>
+      <c r="C10" s="7">
+        <f>IF(B10&lt;SUM(E10:S10),SUM(E10:S10),B10)</f>
+        <v>2</v>
+      </c>
+      <c r="D10" s="8">
+        <f>IF(C10&gt;B10,$C10-(SUM($E10:$S10)),$B10-(SUM($E10:$S10)))</f>
+        <v>0</v>
+      </c>
       <c r="E10" s="12"/>
       <c r="H10" s="13"/>
+      <c r="O10" s="33">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:19" s="32" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
@@ -1676,308 +2284,331 @@
         <v>10</v>
       </c>
       <c r="C11" s="7">
+        <f>IF(B11&lt;SUM(E11:S11),SUM(E11:S11),B11)</f>
+        <v>10</v>
+      </c>
+      <c r="D11" s="8">
+        <f>IF(C11&gt;B11,$C11-(SUM($E11:$S11)),$B11-(SUM($E11:$S11)))</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="H11" s="13"/>
+      <c r="P11" s="32">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="32">
+        <v>2</v>
+      </c>
+      <c r="R11" s="32">
+        <v>2</v>
+      </c>
+      <c r="S11" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="15">
+        <f>SUM(B3:B11)</f>
+        <v>56</v>
+      </c>
+      <c r="C12" s="16">
+        <f>SUM(C3:C11)</f>
+        <v>56</v>
+      </c>
+      <c r="D12" s="16">
+        <f>SUM(D3:D7)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="17">
+        <f>SUM(E3:E7)</f>
+        <v>4</v>
+      </c>
+      <c r="F12" s="17">
+        <f>SUM(F3:F7)</f>
+        <v>2</v>
+      </c>
+      <c r="G12" s="17">
+        <f>SUM(G3:G7)</f>
+        <v>4</v>
+      </c>
+      <c r="H12" s="17">
+        <f>SUM(H3:H7)</f>
+        <v>8</v>
+      </c>
+      <c r="I12" s="17">
+        <f>SUM(I3:I7)</f>
+        <v>2</v>
+      </c>
+      <c r="J12" s="17">
+        <f>SUM(J3:J7)</f>
+        <v>6</v>
+      </c>
+      <c r="K12" s="17">
+        <f>SUM(K3:K7)</f>
+        <v>4</v>
+      </c>
+      <c r="L12" s="17">
+        <f>SUM(L3:L7)</f>
+        <v>2</v>
+      </c>
+      <c r="M12" s="17">
+        <f>SUM(M3:M11)</f>
+        <v>4</v>
+      </c>
+      <c r="N12" s="17">
+        <f>SUM(N3:N11)</f>
+        <v>4</v>
+      </c>
+      <c r="O12" s="17">
+        <f>SUM(O3:O11)</f>
+        <v>4</v>
+      </c>
+      <c r="P12" s="17">
+        <f>SUM(P3:P11)</f>
+        <v>4</v>
+      </c>
+      <c r="Q12" s="17">
+        <f>SUM(Q3:Q11)</f>
+        <v>2</v>
+      </c>
+      <c r="R12" s="17">
+        <f>SUM(R3:R11)</f>
+        <v>2</v>
+      </c>
+      <c r="S12" s="17">
+        <f>SUM(S3:S11)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="19">
+        <v>100</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22">
+        <v>4</v>
+      </c>
+      <c r="F13" s="23">
+        <v>2</v>
+      </c>
+      <c r="G13" s="23">
+        <v>4</v>
+      </c>
+      <c r="H13" s="23">
+        <v>8</v>
+      </c>
+      <c r="I13" s="23">
+        <v>4</v>
+      </c>
+      <c r="J13" s="23">
+        <v>4</v>
+      </c>
+      <c r="K13" s="23">
+        <v>4</v>
+      </c>
+      <c r="L13" s="23">
+        <v>4</v>
+      </c>
+      <c r="M13" s="23">
+        <v>4</v>
+      </c>
+      <c r="N13" s="23">
+        <v>4</v>
+      </c>
+      <c r="O13" s="23">
+        <v>4</v>
+      </c>
+      <c r="P13" s="23">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="23">
+        <v>2</v>
+      </c>
+      <c r="R13" s="23">
+        <v>2</v>
+      </c>
+      <c r="S13" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="27">
+        <f>B12</f>
+        <v>56</v>
+      </c>
+      <c r="E14" s="28">
+        <f t="shared" ref="E14:S14" si="0">D14-E13</f>
+        <v>52</v>
+      </c>
+      <c r="F14" s="28">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="G14" s="28">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="H14" s="28">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="I14" s="28">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="J14" s="28">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="K14" s="28">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="L14" s="28">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="M14" s="28">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="N14" s="28">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="O14" s="28">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D11" s="8">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="1:19" s="33" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="40"/>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
+      <c r="P14" s="28">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B13" s="15">
-        <f>SUM(B3:B11)</f>
-        <v>50</v>
-      </c>
-      <c r="C13" s="16">
-        <f t="shared" ref="C13:S13" si="2">SUM(C3:C7)</f>
-        <v>30</v>
-      </c>
-      <c r="D13" s="16">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="E13" s="17">
-        <f t="shared" si="2"/>
+      <c r="Q14" s="28">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F13" s="17">
-        <f t="shared" si="2"/>
+      <c r="R14" s="28">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G13" s="17">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="H13" s="17">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="I13" s="17">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J13" s="17">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="K13" s="17">
-        <f t="shared" si="2"/>
+      <c r="S14" s="29">
+        <f t="shared" si="0"/>
         <v>0</v>
-      </c>
-      <c r="L13" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R13" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S13" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="19">
-        <f>B13-SUM(E14:R14)</f>
-        <v>2</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22">
-        <v>4</v>
-      </c>
-      <c r="F14" s="23">
-        <v>2</v>
-      </c>
-      <c r="G14" s="23">
-        <v>2</v>
-      </c>
-      <c r="H14" s="23">
-        <v>8</v>
-      </c>
-      <c r="I14" s="23">
-        <v>4</v>
-      </c>
-      <c r="J14" s="23">
-        <v>2</v>
-      </c>
-      <c r="K14" s="23">
-        <v>2</v>
-      </c>
-      <c r="L14" s="23">
-        <v>2</v>
-      </c>
-      <c r="M14" s="23">
-        <v>2</v>
-      </c>
-      <c r="N14" s="23">
-        <v>2</v>
-      </c>
-      <c r="O14" s="23">
-        <v>8</v>
-      </c>
-      <c r="P14" s="23">
-        <v>6</v>
-      </c>
-      <c r="Q14" s="23">
-        <v>2</v>
-      </c>
-      <c r="R14" s="23">
-        <v>2</v>
-      </c>
-      <c r="S14" s="23">
-        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="26" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D15" s="27">
-        <f>B13</f>
+        <f>C12</f>
+        <v>56</v>
+      </c>
+      <c r="E15" s="27">
+        <f>$C$12-SUM(E$3:E$11)</f>
+        <v>52</v>
+      </c>
+      <c r="F15" s="27">
+        <f>E15-SUM(F3:F11)</f>
         <v>50</v>
       </c>
-      <c r="E15" s="28">
-        <f t="shared" ref="E15:S15" si="3">D15-E14</f>
+      <c r="G15" s="27">
+        <f>F15-SUM(G3:G11)</f>
         <v>46</v>
       </c>
-      <c r="F15" s="28">
-        <f t="shared" si="3"/>
-        <v>44</v>
-      </c>
-      <c r="G15" s="28">
-        <f t="shared" si="3"/>
-        <v>42</v>
-      </c>
-      <c r="H15" s="28">
-        <f t="shared" si="3"/>
-        <v>34</v>
-      </c>
-      <c r="I15" s="28">
-        <f t="shared" si="3"/>
+      <c r="H15" s="27">
+        <f>G15-SUM(H3:H11)</f>
+        <v>38</v>
+      </c>
+      <c r="I15" s="27">
+        <f>H15-SUM(I3:I11)</f>
+        <v>36</v>
+      </c>
+      <c r="J15" s="27">
+        <f>I15-SUM(J3:J11)</f>
         <v>30</v>
       </c>
-      <c r="J15" s="28">
-        <f t="shared" si="3"/>
-        <v>28</v>
-      </c>
-      <c r="K15" s="28">
-        <f t="shared" si="3"/>
+      <c r="K15" s="27">
+        <f>J15-SUM(K3:K7)</f>
         <v>26</v>
       </c>
-      <c r="L15" s="28">
-        <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-      <c r="M15" s="28">
-        <f t="shared" si="3"/>
+      <c r="L15" s="27">
+        <f>K15-SUM(L3:L11)</f>
         <v>22</v>
       </c>
-      <c r="N15" s="28">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="O15" s="28">
-        <f t="shared" si="3"/>
+      <c r="M15" s="27">
+        <f>L15-SUM(M3:M11)</f>
+        <v>18</v>
+      </c>
+      <c r="N15" s="27">
+        <f>M15-SUM(N3:N11)</f>
+        <v>14</v>
+      </c>
+      <c r="O15" s="27">
+        <f>N15-SUM(O3:O11)</f>
+        <v>10</v>
+      </c>
+      <c r="P15" s="27">
+        <f>O15-SUM(P3:P11)</f>
+        <v>6</v>
+      </c>
+      <c r="Q15" s="27">
+        <f>P15-SUM(Q3:Q11)</f>
+        <v>4</v>
+      </c>
+      <c r="R15" s="27">
+        <f>Q15-SUM(R3:R11)</f>
+        <v>2</v>
+      </c>
+      <c r="S15" s="27">
+        <f>R15-SUM(S3:S11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="P15" s="28">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="Q15" s="28">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="R15" s="28">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="S15" s="29">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="27">
-        <f>C13</f>
-        <v>30</v>
-      </c>
-      <c r="E16" s="27">
-        <f>$C$13-SUM(E$3:E$7)</f>
-        <v>26</v>
-      </c>
-      <c r="F16" s="27">
-        <f t="shared" ref="F16:S16" si="4">E16-SUM(F3:F7)</f>
-        <v>24</v>
-      </c>
-      <c r="G16" s="27">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="H16" s="27">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="I16" s="27">
-        <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="J16" s="27">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="K16" s="27">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="L16" s="27">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="M16" s="27">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="N16" s="27">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="O16" s="27">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="P16" s="27">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="Q16" s="27">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="R16" s="27">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="S16" s="27">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
     </row>
     <row r="17" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
-        <v>12</v>
+      <c r="A17" s="36" t="s">
+        <v>13</v>
       </c>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
@@ -1997,27 +2628,8 @@
       <c r="R17" s="30"/>
       <c r="S17" s="30"/>
     </row>
-    <row r="18" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="30"/>
-      <c r="S18" s="30"/>
+    <row r="18" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="31"/>
     </row>
     <row r="19" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="31"/>
@@ -2199,116 +2811,173 @@
     <row r="78" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="31"/>
     </row>
-    <row r="79" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A79" s="31"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
+    <mergeCell ref="A16:D16"/>
     <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
   </mergeCells>
-  <conditionalFormatting sqref="A15:S16">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="lessThan">
+  <conditionalFormatting sqref="A14:S15">
+    <cfRule type="cellIs" dxfId="35" priority="25" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+  <conditionalFormatting sqref="A13">
+    <cfRule type="cellIs" dxfId="34" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+  <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="33" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="lessThan">
+  <conditionalFormatting sqref="C13">
+    <cfRule type="cellIs" dxfId="32" priority="28" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:S8">
+  <conditionalFormatting sqref="E3:S5 E7:S7">
+    <cfRule type="cellIs" dxfId="31" priority="29" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D5 D7">
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="cellIs" dxfId="28" priority="32" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="cellIs" dxfId="27" priority="33" operator="greaterThan">
+      <formula>8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="26" priority="34" operator="greaterThan">
+      <formula>8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D5 D7">
+    <cfRule type="cellIs" dxfId="25" priority="35" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D5 D7">
+    <cfRule type="cellIs" dxfId="24" priority="36" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9:S9">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:S11">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6:S6">
     <cfRule type="cellIs" dxfId="15" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D8">
+  <conditionalFormatting sqref="D6">
     <cfRule type="cellIs" dxfId="14" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="greaterThan">
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="greaterThan">
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="greaterThan">
-      <formula>8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="10" priority="18" operator="greaterThan">
-      <formula>8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D8">
-    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
+  <conditionalFormatting sqref="E8:S8">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D8">
-    <cfRule type="cellIs" dxfId="8" priority="20" operator="lessThan">
+  <conditionalFormatting sqref="D8">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9:S10">
+  <conditionalFormatting sqref="D8">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:S10">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9:D10">
+  <conditionalFormatting sqref="D10">
     <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9:D10">
+  <conditionalFormatting sqref="D10">
     <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9:D10">
+  <conditionalFormatting sqref="D10">
     <cfRule type="cellIs" dxfId="4" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11:S12">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11:D12">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11:D12">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11:D12">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A18" r:id="rId1"/>
+    <hyperlink ref="A17" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>

</xml_diff>